<commit_message>
Modfied Bug reports and Test Cases
</commit_message>
<xml_diff>
--- a/Implementation/Api Testing/Api Test Cases.xlsx
+++ b/Implementation/Api Testing/Api Test Cases.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3740ad196387741e/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\college\Github\ecommerce-ui-testing\Implementation\Api Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{A786BA2C-9B05-48CF-92D1-0AB9E9F8C219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A14CFC1-BD46-4038-A34D-8F11FE63918A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A927A5-126F-497D-980B-56686DD9AE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tc4&amp;TC7" sheetId="1" r:id="rId1"/>
     <sheet name="TC13&amp;TC3&amp;TC8" sheetId="2" r:id="rId2"/>
     <sheet name="TC11&amp;TC1&amp;TC6" sheetId="3" r:id="rId3"/>
+    <sheet name="TC10&amp;TC5" sheetId="4" r:id="rId4"/>
+    <sheet name="TC9&amp;TC14" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="356">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -2194,12 +2196,540 @@
   <si>
     <t>Send Get request to search product API not allowed with Query parameter</t>
   </si>
+  <si>
+    <t>AC014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Login API </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Email + Invalid Password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- Add invalid email and password
+5- Click Send </t>
+  </si>
+  <si>
+    <t>email=kariim15@gmail.com
+password=w12a3
+URL: https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can not login</t>
+  </si>
+  <si>
+    <t>invalid email and password (invalid)</t>
+  </si>
+  <si>
+    <t>Response Code=404
+Message="User not found!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Response Code=404
+Message="User not found!" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response Code=404
+Message="User not found!" </t>
+  </si>
+  <si>
+    <t>AC015</t>
+  </si>
+  <si>
+    <t>Valid Email + Invalid Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- Add valid email 
+5-enter invalid password
+6- Click Send </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> email=karim12@gamil.com
+password=w12a3  
+https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t>login fails because wrong password</t>
+  </si>
+  <si>
+    <t>valid email and invalid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Response Code=401
+Message="User not found!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response Code=401
+Message="Unauthorized" </t>
+  </si>
+  <si>
+    <t>Response Code=400
+Message="Bad Request"</t>
+  </si>
+  <si>
+    <t>AC016</t>
+  </si>
+  <si>
+    <t>Invalid Email + Valid Password</t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- enter invalid email 
+5-enter valid password
+6- Click Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email=kariim15@gmail.com
+password=wa12
+https://automationexercise.com/api/verifyLogin
+</t>
+  </si>
+  <si>
+    <t>login fails because wrong email</t>
+  </si>
+  <si>
+    <t>invalid email , valid password</t>
+  </si>
+  <si>
+    <t>Response Code=401
+Message="User not found!"</t>
+  </si>
+  <si>
+    <t>Response Code=401
+Message="Unauthorized"</t>
+  </si>
+  <si>
+    <t>AC017</t>
+  </si>
+  <si>
+    <t>Missing Email Parameter</t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- Remove paramter email 
+5-enter valid password
+6- Click Send</t>
+  </si>
+  <si>
+    <t>email=karm12gmail.com
+password=w12a3
+URL: https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t>login fails because missing paramter email</t>
+  </si>
+  <si>
+    <t>email only</t>
+  </si>
+  <si>
+    <t>Response Code=400
+Message="Bad Request, email parameter is missing"</t>
+  </si>
+  <si>
+    <t>AC018</t>
+  </si>
+  <si>
+    <t>Blank Email</t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4-  email=empty 
+5-enter valid password
+6- Click Send</t>
+  </si>
+  <si>
+    <t>email=
+password=w12a3
+URL: https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login fails because there is no email entered </t>
+  </si>
+  <si>
+    <t>blank email</t>
+  </si>
+  <si>
+    <t>Response Code=400
+Message="Bad Request, email is blank"</t>
+  </si>
+  <si>
+    <t>AC019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blank Password                                         </t>
+  </si>
+  <si>
+    <t>1-- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4-  enter email
+5-password blank
+6- Click Send</t>
+  </si>
+  <si>
+    <t>email=karim12@gmail.com
+password=
+URL: https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t>login fails because there is no entered password</t>
+  </si>
+  <si>
+    <t>blank password</t>
+  </si>
+  <si>
+    <t>Response Code=400
+Message="Bad Request, password is blank"</t>
+  </si>
+  <si>
+    <t>AC020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong HTTP Method </t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to GET
+3- Enter Correct URL
+4- enter valid email
+5-enter password
+6- Click Send</t>
+  </si>
+  <si>
+    <t>email=karim12@gmail.com
+password=wa12
+URL: https://automationexercise.com/api/verifyLogin</t>
+  </si>
+  <si>
+    <t>login fails because wrong method</t>
+  </si>
+  <si>
+    <t>wrong method</t>
+  </si>
+  <si>
+    <t>Response Code=405
+Message="Method Not Allowed"</t>
+  </si>
+  <si>
+    <t>Response Code=200
+Message="OK"</t>
+  </si>
+  <si>
+    <t>AC07</t>
+  </si>
+  <si>
+    <t>Verify Search Product</t>
+  </si>
+  <si>
+    <t>Send request with query parameters</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to GET3- Enter Correct URL4- Enter query parameters5- Click Send</t>
+  </si>
+  <si>
+    <t>Query Parametershttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Send GET Request to product lists API is not allowed with query parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">query parameters
+</t>
+  </si>
+  <si>
+    <t>Response Status Code=400 
+Bad Request</t>
+  </si>
+  <si>
+    <t>Response Status=200
+Response body= contains all searched products list</t>
+  </si>
+  <si>
+    <t>AC08</t>
+  </si>
+  <si>
+    <t>Send Post request for search api</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to POST3- Enter Correct URL4- Enter search_product parameter5- Click Send</t>
+  </si>
+  <si>
+    <t>search_product=jeanshttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Send Post Request for search API with search_parameter query and correct URL</t>
+  </si>
+  <si>
+    <t>search_product=jeans</t>
+  </si>
+  <si>
+    <t>Response Status Code=200
+Response Message=
+"Bad Request, search_product parameter is missing in POST Request""</t>
+  </si>
+  <si>
+    <t>Response Status Code=200 and Response body contains all searched products list</t>
+  </si>
+  <si>
+    <t>Response Status=200 
+BodyMessage=
+"Bad Request"</t>
+  </si>
+  <si>
+    <t>AC09</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to POST3- Enter Incorrect URL4- Enter search_product parameter5- Click Send</t>
+  </si>
+  <si>
+    <t>search_product=tshirthttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Check response for invalid URL</t>
+  </si>
+  <si>
+    <t>search_product=tshirt</t>
+  </si>
+  <si>
+    <t>Response Status Code=405Body response code=405</t>
+  </si>
+  <si>
+    <t>Response Status Code=405 Body response code=405</t>
+  </si>
+  <si>
+    <t>Response Status=200 Body response=405</t>
+  </si>
+  <si>
+    <t>AC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Send request without query parameter</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to POST3- Enter Correct URL4- Click Send</t>
+  </si>
+  <si>
+    <t>No Parametershttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Send POST without search_product parameter</t>
+  </si>
+  <si>
+    <t>Response Status Code=400
+Body Response Code=400
+Message="Bad request, search_product parameter is missing in POST Request"</t>
+  </si>
+  <si>
+    <t>same as Response</t>
+  </si>
+  <si>
+    <t>Response Status Code=200Body Response Code=400Message still missing parameter</t>
+  </si>
+  <si>
+    <t>AC11</t>
+  </si>
+  <si>
+    <t>Send request with blank query parameter</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to POST3- Enter Correct URL4- Blank search_product5- Click Send</t>
+  </si>
+  <si>
+    <t>search_product = ""https://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Send blank search parameter</t>
+  </si>
+  <si>
+    <t>blank parameter</t>
+  </si>
+  <si>
+    <t>Response Status Code=400
+ Bad Request</t>
+  </si>
+  <si>
+    <t>Response Status Code=400 Bad Request</t>
+  </si>
+  <si>
+    <t>AC12</t>
+  </si>
+  <si>
+    <t>Send request with missing headers</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to GET3- Enter Correct URL4- Remove headers5- Click Send</t>
+  </si>
+  <si>
+    <t>No headershttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Check API behavior for missing headers</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>AC13</t>
+  </si>
+  <si>
+    <t>Send POST request with body</t>
+  </si>
+  <si>
+    <t>1- Open Postman2- Set Method to POST3- Enter Correct URL4- Enter search_parameter5- Enter body6- Click Send</t>
+  </si>
+  <si>
+    <t>Body: {"Age"=20}search_product=jeanshttps://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Send POST with body and parameter</t>
+  </si>
+  <si>
+    <t>Body + parameter</t>
+  </si>
+  <si>
+    <t>AC14</t>
+  </si>
+  <si>
+    <t>No Token send</t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- Enter search_product parameter
+5- Remove auth token
+6- Click Send</t>
+  </si>
+  <si>
+    <t>search_product=jeans
+https://automationexercise.com/api/searchProduct</t>
+  </si>
+  <si>
+    <t>Check response for unauthorized access</t>
+  </si>
+  <si>
+    <t>no auth token</t>
+  </si>
+  <si>
+    <t>Response Status Code=401
+Message="Unauthorized"</t>
+  </si>
+  <si>
+    <t>AC15</t>
+  </si>
+  <si>
+    <t>Valid Search with Correct Data</t>
+  </si>
+  <si>
+    <t>1- Open Postman
+2- Set Method to POST
+3- Enter Correct URL
+4- Enter valid search_product
+5- Click Send</t>
+  </si>
+  <si>
+    <t>Verify successful search</t>
+  </si>
+  <si>
+    <t>valid search</t>
+  </si>
+  <si>
+    <t>Response Status Code=200
+Message="Products found</t>
+  </si>
+  <si>
+    <t>Response Status Code=200
+Message="Products found"</t>
+  </si>
+  <si>
+    <t>API-9-DEL-VERIFY-LOGIN</t>
+  </si>
+  <si>
+    <t>Verify that the API successfully deletes the verification record of a logged-in user.</t>
+  </si>
+  <si>
+    <t>Ensure the API deletes the login verification entry when a valid request is sent.</t>
+  </si>
+  <si>
+    <t>1. Send DELETE request
+2. Add Authorization token
+3. Provide User ID
+4. Send request
+5. Validate response</t>
+  </si>
+  <si>
+    <t>Authorization: Bearer valid-token-123; UserID: 78945</t>
+  </si>
+  <si>
+    <t>Confirm the system deletes the verification login entry with valid authentication.</t>
+  </si>
+  <si>
+    <t>DELETE /api/v1/auth/verify-login/{userId}</t>
+  </si>
+  <si>
+    <t>{"message": "Verification login deleted successfully", "status": true}</t>
+  </si>
+  <si>
+    <t>Status 200 and deletion confirmation message</t>
+  </si>
+  <si>
+    <t>API-14-GET-USER-EMAIL</t>
+  </si>
+  <si>
+    <t>Verify that the API retrieves complete user details using a valid email.</t>
+  </si>
+  <si>
+    <t>Ensure the system returns the correct user account information for a valid email.</t>
+  </si>
+  <si>
+    <t>1. Send GET request
+2. Provide valid email
+3. Add Authorization token
+4. Send request
+5. Validate response</t>
+  </si>
+  <si>
+    <t>Email: testuser@example.com; Authorization: Bearer valid-token-123</t>
+  </si>
+  <si>
+    <t>Ensure the API retrieves correct user account details such as name, email, phone, and status.</t>
+  </si>
+  <si>
+    <t>GET /api/v1/users/details?email=testuser@example.com</t>
+  </si>
+  <si>
+    <t>{"email": "testuser@example.com", "fullName": "Test User", "phone": "0100000000"}</t>
+  </si>
+  <si>
+    <t>Status 200 and return of full user record</t>
+  </si>
+  <si>
+    <t>500 error returned, record not deleted</t>
+  </si>
+  <si>
+    <t>Missing fields: phone, status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2265,8 +2795,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2303,6 +2841,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2332,7 +2882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2385,6 +2935,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2401,10 +2969,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2727,7 +3291,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="27" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
@@ -3552,7 +4116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98004F06-D0A4-4507-AE3D-610C71468CD9}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+    <sheetView zoomScale="82" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4017,4 +4581,734 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9C9C78-1F65-4D04-823E-17AD06A15873}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="43" style="8" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="35.5546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="30.109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="22" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://automationexercise.com/api/searchProduct" xr:uid="{104DC537-6F0E-4BFE-A1F9-F4AE20E5EE74}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://automationexercise.com/api/searchProduct" xr:uid="{F03652ED-3F7B-473F-9FEB-0F1AF62A0620}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://automationexercise.com/api/searchProduct" xr:uid="{B3F4A94D-5781-4589-9C8F-16B9B0554086}"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://automationexercise.com/api/searchProduct" xr:uid="{05E23037-F440-4219-BF1F-E800E41A3A04}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://automationexercise.com/api/searchProduct" xr:uid="{DE52B3EF-AC66-4758-96BD-C1D0D7BF8C2C}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://automationexercise.com/api/searchProduct" xr:uid="{45C785FA-CC1D-46A6-874D-874B61022FD9}"/>
+    <hyperlink ref="E8" r:id="rId7" display="https://automationexercise.com/api/searchProduct" xr:uid="{B89B59BF-93F9-426F-AEA9-8EA854D1DA9F}"/>
+    <hyperlink ref="E13" r:id="rId8" display="email=kariim15@gmail.com_x000a_password=wa12_x000a__x000a_" xr:uid="{FE7FFE1D-EDBD-4D94-B696-24BFE7521FD2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA4E6D-5C67-4B5A-B30B-55021719F408}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="79.109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="74.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="99.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="81.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="93.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="73.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="77" style="8" customWidth="1"/>
+    <col min="9" max="9" width="56.6640625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="45.109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modfied Api Bug reports and Test Cases
</commit_message>
<xml_diff>
--- a/Implementation/Api Testing/Api Test Cases.xlsx
+++ b/Implementation/Api Testing/Api Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\college\Github\ecommerce-ui-testing\Implementation\Api Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A927A5-126F-497D-980B-56686DD9AE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698B75F7-C5CE-44FE-9F4E-F433B48D9C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tc4&amp;TC7" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="TC11&amp;TC1&amp;TC6" sheetId="3" r:id="rId3"/>
     <sheet name="TC10&amp;TC5" sheetId="4" r:id="rId4"/>
     <sheet name="TC9&amp;TC14" sheetId="5" r:id="rId5"/>
+    <sheet name="TC12&amp;TC2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="411">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -2724,12 +2725,1571 @@
   <si>
     <t>Missing fields: phone, status</t>
   </si>
+  <si>
+    <t>DA01</t>
+  </si>
+  <si>
+    <t>verify delete account</t>
+  </si>
+  <si>
+    <t>send Delete request to
+ account API to get correct endpoint</t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to delete
+3- Enter correct URL
+4- Open Scibts tab
+5-Enter qurrey parametar
+6-Click Post response tab
+7-Write javaScript Assertion
+8-Click Send</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>URL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  https://automationexercise.com/api/deleteAccount
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> javaScript Assertion: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pm.test("Status code is 200", function(){
+   pm.response.to.have.status(200); });
+pm.test("Account deleted!", function () { pm.expect(pm.response.json().message).to.eql("Account deleted!");});
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>param key1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Email
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>param key2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>param value1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ammarkhaled632@GMAIL.COM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>param value2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z7sxmXFbhDgY@jS</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Send delete Request to Accounts 
+API with correct URL </t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 400,
+    "message": "Bad request, email parameter is missing in DELETE request."
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Account deleted!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Body responseCode:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 400,
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bad request, email parameter is missing in DELETE request."</t>
+    </r>
+  </si>
+  <si>
+    <t>DA02</t>
+  </si>
+  <si>
+    <t>send Delete request to
+ account API to get incorrect endpoint</t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to delete
+3- Enter incorrect URL
+4-Click Send</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">URL: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+https://automationexercise.com/aspi/deleteAccount</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Send delete Request to Accounts 
+API with incorrect URL </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 404
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Not Found"</t>
+    </r>
+  </si>
+  <si>
+    <t>DA03</t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to delete
+3- Enter correct URL
+4-Add Body
+5-Click Send</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>URL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://automationexercise.com/api/deleteAccount
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body key1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Email
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body key2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body value1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ammarkhaled632@GMAIL.COM
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body value2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z7sxmXFbhDgY@jS</t>
+    </r>
+  </si>
+  <si>
+    <t>Send delete Request to Accounts 
+API with Body</t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 200,
+    "message": "Account deleted!"
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 400
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bad Request"</t>
+    </r>
+  </si>
+  <si>
+    <t>DA04</t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to delete
+3- Enter correct URL
+4-Add Headers
+5-Click Send</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>URL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://automationexercise.com/api/deleteAccount
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Header:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>application/jason</t>
+    </r>
+  </si>
+  <si>
+    <t>Send delete Request to Accounts 
+API with Header</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 400,
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bad request, email parameter is missing in DELETE request."</t>
+    </r>
+  </si>
+  <si>
+    <t>verify  product 
+list post</t>
+  </si>
+  <si>
+    <t>send post request to
+ product lists API to get incorrect endpoint</t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to post
+3- Enter correct URL
+4- Open Scibts tab
+5-Click Post response tab
+6-Write javaScript Assertion
+7-Click Send</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>URL:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ https://automationexercise.com/api/productsList
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> javaScript Assertion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+pm.test("Status code is 405", function () {
+    pm.response.to.have.status(405);});
+pm.test("Message is Method Not Allowed", function () { pm.expect(pm.response.json().message).to.eql("This request method is not supported.");});</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Send post Request to Product Lists API with correct URL </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 405
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body Response Message:"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This request method
+ is not supported."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 405
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Body Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" This request method
+ is not supported."</t>
+    </r>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to Get
+3- Enter incorrect URL
+4-Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+ https://automationexercise.com/aPPpi/productsList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send post Request to Product Lists API with incorrect URL </t>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to Get
+3- Enter correct URL
+4-Add Body
+5-Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+ https://automationexercise.com/api/productsList
+Body:{ "name":"aber"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send post Request to Product Lists API with Body </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " "responseCode": 200,
+    "products": [
+        {
+            "id": 1,
+            "name": "Blue Top",
+            "price": "Rs. 500",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 2,
+            "name": "Men Tshirt",
+            "price": "Rs. 400",
+            "brand": "H&amp;M",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        },
+        {
+            "id": 3,
+            "name": "Sleeveless Dress",
+            "price": "Rs. 1000",
+            "brand": "Madame",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 4,
+            "name": "Stylish Dress",
+            "price": "Rs. 1500",
+            "brand": "Madame",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 5,
+            "name": "Winter Top",
+            "price": "Rs. 600",
+            "brand": "Mast &amp; Harbour",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 6,
+            "name": "Summer White Top",
+            "price": "Rs. 400",
+            "brand": "H&amp;M",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 7,
+            "name": "Madame Top For Women",
+            "price": "Rs. 1000",
+            "brand": "Madame",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 8,
+            "name": "Fancy Green Top",
+            "price": "Rs. 700",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 11,
+            "name": "Sleeves Printed Top - White",
+            "price": "Rs. 499",
+            "brand": "Babyhug",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 12,
+            "name": "Half Sleeves Top Schiffli Detailing - Pink",
+            "price": "Rs. 359",
+            "brand": "Babyhug",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 13,
+            "name": "Frozen Tops For Kids",
+            "price": "Rs. 278",
+            "brand": "Allen Solly Junior",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 14,
+            "name": "Full Sleeves Top Cherry - Pink",
+            "price": "Rs. 679",
+            "brand": "Kookie Kids",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 15,
+            "name": "Printed Off Shoulder Top - White",
+            "price": "Rs. 315",
+            "brand": "Babyhug",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 16,
+            "name": "Sleeves Top and Short - Blue &amp; Pink",
+            "price": "Rs. 478",
+            "brand": "Babyhug",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 18,
+            "name": "Little Girls Mr. Panda Shirt",
+            "price": "Rs. 1200",
+            "brand": "Kookie Kids",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 19,
+            "name": "Sleeveless Unicorn Patch Gown - Pink",
+            "price": "Rs. 1050",
+            "brand": "Allen Solly Junior",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 20,
+            "name": "Cotton Mull Embroidered Dress",
+            "price": "Rs. 1190",
+            "brand": "Kookie Kids",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 21,
+            "name": "Blue Cotton Indie Mickey Dress",
+            "price": "Rs. 1530",
+            "brand": "Biba",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 22,
+            "name": "Long Maxi Tulle Fancy Dress Up Outfits -Pink",
+            "price": "Rs. 1600",
+            "brand": "Biba",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 23,
+            "name": "Sleeveless Unicorn Print Fit &amp; Flare Net Dress - Multi",
+            "price": "Rs. 1100",
+            "brand": "Biba",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 24,
+            "name": "Colour Blocked Shirt – Sky Blue",
+            "price": "Rs. 849",
+            "brand": "Allen Solly Junior",
+            "category": {
+                "usertype": {
+                    "usertype": "Kids"
+                },
+                "category": "Tops &amp; Shirts"
+            }
+        },
+        {
+            "id": 28,
+            "name": "Pure Cotton V-Neck T-Shirt",
+            "price": "Rs. 1299",
+            "brand": "H&amp;M",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        },
+        {
+            "id": 29,
+            "name": "Green Side Placket Detail T-Shirt",
+            "price": "Rs. 1000",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        },
+        {
+            "id": 30,
+            "name": "Premium Polo T-Shirts",
+            "price": "Rs. 1500",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        },
+        {
+            "id": 31,
+            "name": "Pure Cotton Neon Green Tshirt",
+            "price": "Rs. 850",
+            "brand": "H&amp;M",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        },
+        {
+            "id": 33,
+            "name": "Soft Stretch Jeans",
+            "price": "Rs. 799",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Jeans"
+            }
+        },
+        {
+            "id": 35,
+            "name": "Regular Fit Straight Jeans",
+            "price": "Rs. 1200",
+            "brand": "H&amp;M",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Jeans"
+            }
+        },
+        {
+            "id": 37,
+            "name": "Grunt Blue Slim Fit Jeans",
+            "price": "Rs. 1400",
+            "brand": "Polo",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Jeans"
+            }
+        },
+        {
+            "id": 38,
+            "name": "Rose Pink Embroidered Maxi Dress",
+            "price": "Rs. 2300",
+            "brand": "Madame",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Dress"
+            }
+        },
+        {
+            "id": 39,
+            "name": "Cotton Silk Hand Block Print Saree",
+            "price": "Rs. 3000",
+            "brand": "Biba",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Saree"
+            }
+        },
+        {
+            "id": 40,
+            "name": "Rust Red Linen Saree",
+            "price": "Rs. 3500",
+            "brand": "Biba",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Saree"
+            }
+        },
+        {
+            "id": 41,
+            "name": "Beautiful Peacock Blue Cotton Linen Saree",
+            "price": "Rs. 5000",
+            "brand": "Madame",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Saree"
+            }
+        },
+        {
+            "id": 42,
+            "name": "Lace Top For Women",
+            "price": "Rs. 1400",
+            "brand": "Mast &amp; Harbour",
+            "category": {
+                "usertype": {
+                    "usertype": "Women"
+                },
+                "category": "Tops"
+            }
+        },
+        {
+            "id": 43,
+            "name": "GRAPHIC DESIGN MEN T SHIRT - BLUE",
+            "price": "Rs. 1389",
+            "brand": "Mast &amp; Harbour",
+            "category": {
+                "usertype": {
+                    "usertype": "Men"
+                },
+                "category": "Tshirts"
+            }
+        }
+    ]
+}"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 400
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bad Request"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " "responseCode": 200 and accept Body</t>
+    </r>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to Get
+3- Enter correct URL
+4-Add Params
+5-Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+ https://automationexercise.com/api/productsList
+param key: Password
+param value:1234</t>
+  </si>
+  <si>
+    <t>Send post Request to Product Lists API with params</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " "responseCode": 200 and accept params</t>
+    </r>
+  </si>
+  <si>
+    <t>1-Open postman
+2-Set Method to Get
+3- Enter correct URL
+4-Add Headers
+5-Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+ https://automationexercise.com/api/productsList
+Header:application/jason</t>
+  </si>
+  <si>
+    <t>Send post Request to Product Lists API with Headers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 200
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Response Message:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " "responseCode": 200 and accept Headers</t>
+    </r>
+  </si>
+  <si>
+    <t>PR01</t>
+  </si>
+  <si>
+    <t>PR02</t>
+  </si>
+  <si>
+    <t>PR03</t>
+  </si>
+  <si>
+    <t>PR04</t>
+  </si>
+  <si>
+    <t>PR05</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2803,8 +4363,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2853,6 +4451,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2882,7 +4486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2951,6 +4555,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5183,7 +6817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EA4E6D-5C67-4B5A-B30B-55021719F408}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -5311,4 +6945,430 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C338577-27F8-4153-A7C9-10A491691330}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="32" style="8" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="31.5546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="22.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="226.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="121.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="121.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="191.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>408</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>397</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>405</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modfied Api postman test cases and files
</commit_message>
<xml_diff>
--- a/Implementation/Api Testing/Api Test Cases.xlsx
+++ b/Implementation/Api Testing/Api Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\college\Github\ecommerce-ui-testing\Implementation\Api Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698B75F7-C5CE-44FE-9F4E-F433B48D9C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9E7C50-5A0D-483B-956F-F499D8836051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{369F8B14-4858-4B02-9C36-1CB6A84B67AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tc4&amp;TC7" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="513">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -4284,12 +4284,685 @@
   <si>
     <t>PR05</t>
   </si>
+  <si>
+    <t>Register User Account with valid data</t>
+  </si>
+  <si>
+    <t>Send post request to register API with valid data and correct end point</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5. Add valid body params
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json</t>
+  </si>
+  <si>
+    <t>Send post request to register API with valid data</t>
+  </si>
+  <si>
+    <t>{"responseCode": 201, "message": "User created!"}</t>
+  </si>
+  <si>
+    <t>Response Code: 200
+ "message": "User created!"</t>
+  </si>
+  <si>
+    <t>Response Code: 200
+{"responseCode": 201, "message": "User created!"}</t>
+  </si>
+  <si>
+    <t>Send post request to register API with existing email</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5-add valid body parameters
+6. re enter the same email
+7. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+body with the same email</t>
+  </si>
+  <si>
+    <t>Send post request to register API with existing email are not allowed</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Email already exists!"}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: "Email already exists"</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: "Email already exists"</t>
+  </si>
+  <si>
+    <t>Send post request to register API  without name</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5-add valid body parameters without name
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+body without name</t>
+  </si>
+  <si>
+    <t>Send post request to register API without name are not allowed</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Bad request, name parameter is missing in POST request."}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, name parameter is missing in POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, name parameter is missing in POST request
+"</t>
+  </si>
+  <si>
+    <t>Send post request to register API without email</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5-add valid body parameters without email
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+body without email</t>
+  </si>
+  <si>
+    <t>Send post request to register API without email are not allowed</t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 400,
+    "message": "Bad request, email parameter is missing in POST request."
+}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, email parameter is missing in POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, email parameter is missing in POST request
+"</t>
+  </si>
+  <si>
+    <t>Send post request to register API without password</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5-add valid body parameters without pasword
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+body without password</t>
+  </si>
+  <si>
+    <t>Send post request to register API without password are not allowed</t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 400,
+    "message": "Bad request, password parameter is missing in POST request."
+}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, password parameter is missing in POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, password parameter is missing in POST request
+"</t>
+  </si>
+  <si>
+    <t>Send post request to register API with empty body</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to POST
+3. Enter correct URL
+4. Add headers
+5. Click Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+</t>
+  </si>
+  <si>
+    <t>Send post request to register API without body are not allowed</t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 400,
+    "message": "Bad request, name parameter is missing in POST request."
+}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, body is required in POST request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send Get request to register API </t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to GET
+3. Enter correct URL
+4. Add headers
+5. Add valid body params
+6. Click Send</t>
+  </si>
+  <si>
+    <t>Send Get request to register API are not allowed</t>
+  </si>
+  <si>
+    <t>Response state code : 405 
+Message:"Method \"GET\" not allowed"</t>
+  </si>
+  <si>
+    <t>Send post request to register API with incorrect end Point</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter incorrect URL
+4. Add headers
+5. Add valid body params
+6. Click Send</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL:
+https://automationexercise.com/api/createAccounttt
+Headers: Content-Type: application/json
+</t>
+  </si>
+  <si>
+    <t>Send post request to register API with incorrect end Point are not allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+&lt;head&gt;
+  &lt;meta http-equiv="content-type" content="text/html; charset=utf-8"&gt;
+  &lt;title&gt;Page not found at /api/createAccounttt&lt;/title&gt;
+  &lt;meta name="robots" content="NONE,NOARCHIVE"&gt;
+  &lt;style type="text/css"&gt;
+    html * { padding: 0; margin: 0;
+}
+    body * { padding: 10px 20px;
+}
+    body * * { padding: 0;
+}
+    body { font:small sans-serif; background:#eee; color:#000;
+}
+    body&gt;div { border-bottom: 1px solid #ddd;
+}
+    h1 { font-weight:normal; margin-bottom:.4em;
+}
+    h1 span { font-size: 60%; color:#666; font-weight:normal;
+}
+    table { border:none; border-collapse: collapse; width: 100%;
+}
+    td, th { vertical-align:top; padding: 2px 3px;
+}
+    th { width:12em; text-align:right; color:#666; padding-right:.5em;
+}
+    #info { background:#f6f6f6;
+}
+    #info ol { margin: 0.5em 4em;
+}
+    #info ol li { font-family: monospace;
+}
+    #summary { background: #ffc;
+}
+    #explanation { background:#eee; border-bottom: 0px none;
+}
+    pre.exception_value { font-family: sans-serif; color: #575757; font-size: 1.5em; margin: 10px 0 10px 0;
+}
+  &lt;/style&gt;
+&lt;/head&gt;
+&lt;body&gt;
+  &lt;div id="summary"&gt;
+    &lt;h1&gt;Page not found &lt;span&gt;(404)&lt;/span&gt;&lt;/h1&gt;
+    &lt;table class="meta"&gt;
+      &lt;tr&gt;
+        &lt;th&gt;Request Method:&lt;/th&gt;
+        &lt;td&gt;POST&lt;/td&gt;
+      &lt;/tr&gt;
+      &lt;tr&gt;
+        &lt;th&gt;Request URL:&lt;/th&gt;
+        &lt;td&gt;https: //automationexercise.com/api/createAccounttt&lt;/td&gt;
+      &lt;/tr&gt;
+    &lt;/table&gt;
+  &lt;/div&gt;
+  &lt;div id="info"&gt;
+      &lt;p&gt;
+      Using the URLconf defined in &lt;code&gt;automation_exercise.urls&lt;/code&gt;,
+      Django tried these URL patterns, in this order:
+      &lt;/p&gt;
+      &lt;ol&gt;
+          &lt;li&gt;
+                admin/
+          &lt;/li&gt;
+          &lt;li&gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                get_product_picture/&amp;lt;int:product_id&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                product_details/&amp;lt;int:product_id&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                products
+          &lt;/li&gt;
+          &lt;li&gt;
+                contact_us
+          &lt;/li&gt;
+          &lt;li&gt;
+                add_to_cart/&amp;lt;int:product_id&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                view_cart
+          &lt;/li&gt;
+          &lt;li&gt;
+                delete_cart/&amp;lt;int:product_id&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                login
+          &lt;/li&gt;
+          &lt;li&gt;
+                signup
+          &lt;/li&gt;
+          &lt;li&gt;
+                account_created
+          &lt;/li&gt;
+          &lt;li&gt;
+                logout
+          &lt;/li&gt;
+          &lt;li&gt;
+                checkout
+          &lt;/li&gt;
+          &lt;li&gt;
+                payment
+          &lt;/li&gt;
+          &lt;li&gt;
+                delete_account
+          &lt;/li&gt;
+          &lt;li&gt;
+                brand_products/&amp;lt;str:brand&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                category_products/&amp;lt;int:category_id&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                test_cases
+          &lt;/li&gt;
+          &lt;li&gt;
+                api_list
+          &lt;/li&gt;
+          &lt;li&gt;
+                download_invoice/&amp;lt;int:overall_amount&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                payment_done/&amp;lt;int:overall_amount&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                video_tutorials
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/productsList
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/brandsList
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/searchProduct
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/verifyLogin
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/createAccount
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/deleteAccount
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/updateAccount
+          &lt;/li&gt;
+          &lt;li&gt;
+                api/getUserDetailByEmail
+          &lt;/li&gt;
+          &lt;li&gt;
+                &amp;lt;str:random_string&amp;gt;
+          &lt;/li&gt;
+          &lt;li&gt;
+                ^static/(?P&amp;lt;path&amp;gt;.*)$
+          &lt;/li&gt;
+      &lt;/ol&gt;
+      &lt;p&gt;
+          The current path, &lt;code&gt;api/createAccounttt&lt;/code&gt;,
+        didn’t match any of these.
+      &lt;/p&gt;
+  &lt;/div&gt;
+  &lt;div id="explanation"&gt;
+    &lt;p&gt;
+      You’re seeing this error because you have &lt;code&gt;DEBUG = True&lt;/code&gt; in
+      your Django settings file. Change that to &lt;code&gt;False&lt;/code&gt;, and Django
+      will display a standard 404 page.
+    &lt;/p&gt;
+  &lt;/div&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+</t>
+  </si>
+  <si>
+    <t>Response code:404
+not found</t>
+  </si>
+  <si>
+    <t>Send post request to register API with missing Headers</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. remove Headers
+5. Add valid body params
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+No Headers</t>
+  </si>
+  <si>
+    <t>Send post request to register API without Header are not allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;html&gt;
+&lt;head&gt;&lt;title&gt;400 Bad Request&lt;/title&gt;&lt;/head&gt;
+&lt;body&gt;
+&lt;center&gt;&lt;h1&gt;400 Bad Request&lt;/h1&gt;&lt;/center&gt;
+&lt;hr&gt;&lt;center&gt;cloudflare&lt;/center&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+</t>
+  </si>
+  <si>
+    <t>Response code :400
+Message : "Bad Request"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pass</t>
+  </si>
+  <si>
+    <t>Send post request to register API with wrong parameter name</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add invalid body params
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+Rename email → emails</t>
+  </si>
+  <si>
+    <t>Send post request to register API are not allowed with wrong parameter name</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, name is required in POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, name is required in POST request</t>
+  </si>
+  <si>
+    <t>Faill</t>
+  </si>
+  <si>
+    <t>Send post request to register API with wrong data type</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body params expect biirth_year input it as a string
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+birth_year: "abc"</t>
+  </si>
+  <si>
+    <t>Send post request to register API are not allowed with wrong data type</t>
+  </si>
+  <si>
+    <t>{
+    "responseCode": 201,
+    "message": "User created!"
+}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, characters in Birth day field in POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 201
+Message:"User Created"</t>
+  </si>
+  <si>
+    <t>Send post request to register API withinvalid mobile number formate</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body params expect mobile number input a characters instead of numbers
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+mobile_number: "test"</t>
+  </si>
+  <si>
+    <t>Send post request to register API with invalid mobile number formate are not allowed</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, characters in mobile number field in POST request</t>
+  </si>
+  <si>
+    <t>Send post request to register API with Long name input</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body params and name=300 characters 
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+name=300 characters</t>
+  </si>
+  <si>
+    <t>Send post request to register API are not allowed with Long name input</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, very long name in POST request</t>
+  </si>
+  <si>
+    <t>Send post request to register API with Special character in name</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body params and enter special characters in name field
+6. Click Send</t>
+  </si>
+  <si>
+    <t>URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+name: "@@@@!!!!"</t>
+  </si>
+  <si>
+    <t>Send post request to register API with Special character in name are not allowed</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, special characters in name in POST request</t>
+  </si>
+  <si>
+    <t>Send post request to register API withmissing address1</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body paramswithout address1
+6. Click Send</t>
+  </si>
+  <si>
+    <t>"URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+No Address1</t>
+  </si>
+  <si>
+    <t>Send post request to register API with missing address1 are not allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {
+    "responseCode": 400,
+    "message": "Bad request, address1 parameter is missing in POST request."
+}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, address1 parameter is missingin POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, address1 is missing in POST request</t>
+  </si>
+  <si>
+    <t>Send post request to register API with zipcode missing</t>
+  </si>
+  <si>
+    <t>1. Open Postman
+2. Set method to Post
+3. Enter correct URL
+4. Add Headers
+5. Add valid body paramswithout zipcode
+6. Click Send</t>
+  </si>
+  <si>
+    <t>"URL:
+https://automationexercise.com/api/createAccount
+Headers: Content-Type: application/json
+No Zipcode</t>
+  </si>
+  <si>
+    <t>Send post request to register API with zipcode missing are not allowed</t>
+  </si>
+  <si>
+    <t>{"responseCode": 400, "message": "Bad request, zipcode parameter is missing in POST request."}</t>
+  </si>
+  <si>
+    <t>Response States Code= 400
+Body Response Code = 400
+Message: Bad request, zipcode parameter is missingin POST request</t>
+  </si>
+  <si>
+    <t>Response States Code= 200
+Body Response Code = 400
+Message: Bad request, zipcode is missing in POST request</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4401,6 +5074,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -4486,7 +5172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4586,6 +5272,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5748,10 +6440,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98004F06-D0A4-4507-AE3D-610C71468CD9}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6210,6 +6902,425 @@
       </c>
       <c r="K15" s="16" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B22" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="144" x14ac:dyDescent="0.3">
+      <c r="B24" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>486</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>491</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>496</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>481</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -6951,7 +8062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C338577-27F8-4153-A7C9-10A491691330}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>